<commit_message>
Init all settings tested
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a773611\Documents\UiPath\Sanofi_PDF_Processing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Sanofi UiPath\Solution\Sanofi_PDF_Processing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34637F5-5495-4757-8C44-7E64895B9893}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2349F0CF-0EAD-49DC-B1F7-0A5499311BE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-6495" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -58,22 +58,22 @@
     <t>RU0X</t>
   </si>
   <si>
+    <t>SourceDirectory</t>
+  </si>
+  <si>
+    <t>C:\Users\a773611\Desktop\source\</t>
+  </si>
+  <si>
+    <t>Путь к папке, где размещены исходные файлы (ZIP архивы)</t>
+  </si>
+  <si>
+    <t>02:00:00</t>
+  </si>
+  <si>
     <t>C:\Users\a773611\Desktop\temporary\</t>
   </si>
   <si>
-    <t>TemporaryDirectory</t>
-  </si>
-  <si>
-    <t>SourceDirectory</t>
-  </si>
-  <si>
-    <t>C:\Users\a773611\Desktop\source\</t>
-  </si>
-  <si>
-    <t>Путь к папке, где размещены исходные файлы (ZIP архивы)</t>
-  </si>
-  <si>
-    <t>02:00:00</t>
+    <t>Temporary1Directory</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -458,21 +458,21 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -494,7 +494,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>

</xml_diff>